<commit_message>
Updated HIS test cases and page objects
</commit_message>
<xml_diff>
--- a/TestData/HIS_DATA_WorkBook.xlsx
+++ b/TestData/HIS_DATA_WorkBook.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10013887\Project_AIG\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31FE273-350D-4023-884C-F590D8FEEA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79595A4-7307-4270-96EC-FC9689F17199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
-    <sheet name="Front_Office" sheetId="3" r:id="rId2"/>
+    <sheet name="Front_Office_Registration" sheetId="3" r:id="rId2"/>
     <sheet name="Masters" sheetId="2" r:id="rId3"/>
     <sheet name="Inventory_Options" sheetId="4" r:id="rId4"/>
     <sheet name="Indent_Items" sheetId="5" r:id="rId5"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="243">
   <si>
     <t>Queries</t>
   </si>
@@ -160,18 +160,9 @@
     <t>Success Message</t>
   </si>
   <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Married</t>
-  </si>
-  <si>
     <t>Mafli, house-14-04-03</t>
   </si>
   <si>
-    <t>uppal</t>
-  </si>
-  <si>
     <t>Direct Receipt</t>
   </si>
   <si>
@@ -181,12 +172,6 @@
     <t>HisPassword@1234</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>KiranLal</t>
-  </si>
-  <si>
     <t>option_name</t>
   </si>
   <si>
@@ -226,9 +211,6 @@
     <t>Nikith@4744</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
     <t>item_name</t>
   </si>
   <si>
@@ -236,6 +218,543 @@
   </si>
   <si>
     <t>MICROPORE -2 INCH PLASTER</t>
+  </si>
+  <si>
+    <t>25% DEXTROSE 100ML</t>
+  </si>
+  <si>
+    <t>ADNEON -2ML- INJ</t>
+  </si>
+  <si>
+    <t>ALCOHOL SWABS</t>
+  </si>
+  <si>
+    <t>AMIODON 150MG INJ 3ML</t>
+  </si>
+  <si>
+    <t>ARTACIL 25MG/2.5ML INJ</t>
+  </si>
+  <si>
+    <t>ASTHALIN RESPULES</t>
+  </si>
+  <si>
+    <t>ATORVA 80MG TAB</t>
+  </si>
+  <si>
+    <t>ATRAPURE 25MG /2.5ML INJ</t>
+  </si>
+  <si>
+    <t>AUGPEN-1.2GM-INJ</t>
+  </si>
+  <si>
+    <t>AVIL-2ML-INJ</t>
+  </si>
+  <si>
+    <t>BAIN CIRCUIT- ADULT</t>
+  </si>
+  <si>
+    <t>BAIN CIRCUIT -PAED</t>
+  </si>
+  <si>
+    <t>BAND -AID ROUND</t>
+  </si>
+  <si>
+    <t>BUDECORT-0.5MG-RESPULES</t>
+  </si>
+  <si>
+    <t>CAMERA COVERS- 25CM X 2MTRS</t>
+  </si>
+  <si>
+    <t>CERTOFIX DUO -V715</t>
+  </si>
+  <si>
+    <t>CERTOFIX MONO -V315</t>
+  </si>
+  <si>
+    <t>CLOPITAB 75MG TAB</t>
+  </si>
+  <si>
+    <t>CORT-S 100MG INJ</t>
+  </si>
+  <si>
+    <t>CPRESSIN-P 20IU/1ML INJ</t>
+  </si>
+  <si>
+    <t>CRIMP CAPS</t>
+  </si>
+  <si>
+    <t>C-TRI 1GM-INJ</t>
+  </si>
+  <si>
+    <t>DERIPHYLLIN- 2ML -AMP</t>
+  </si>
+  <si>
+    <t>DEXONA-4MG-INJ</t>
+  </si>
+  <si>
+    <t>DEXTROSE 10% 500ML</t>
+  </si>
+  <si>
+    <t>DEXTROSE 5% 500ML</t>
+  </si>
+  <si>
+    <t>DILZEM 5ML INJ</t>
+  </si>
+  <si>
+    <t>DISCOFIX 10CM EXTENSION</t>
+  </si>
+  <si>
+    <t>DISCOFIX 3 WAY CONNECTOR</t>
+  </si>
+  <si>
+    <t>DNS 500ML FLEXIDRIP</t>
+  </si>
+  <si>
+    <t>DOMIN-INJ</t>
+  </si>
+  <si>
+    <t>DOSIFLOW -REGULATOR</t>
+  </si>
+  <si>
+    <t>DOTAMIN-INJ</t>
+  </si>
+  <si>
+    <t>DUOLIN-RESPULES</t>
+  </si>
+  <si>
+    <t>DUPHALAC -300ML- ENEMA</t>
+  </si>
+  <si>
+    <t>DURAPORE -1 INCH</t>
+  </si>
+  <si>
+    <t>DURAPORE- 3 INCH</t>
+  </si>
+  <si>
+    <t>DYNATROY AQ -1ML- INJ</t>
+  </si>
+  <si>
+    <t>ECOSPRIN-150MG-TAB</t>
+  </si>
+  <si>
+    <t>ELASTIC DYNAPLASTER 10CMX4/6M</t>
+  </si>
+  <si>
+    <t>ENEMA (PROCTLYSIS)</t>
+  </si>
+  <si>
+    <t>ET TUBE 3.5 WITHCUFF-RUSCH</t>
+  </si>
+  <si>
+    <t>ET TUBE- 4.0 -UNCUFFED- PORTEX</t>
+  </si>
+  <si>
+    <t>ET TUBE -4.5 -UNCUFFED- PORTEX</t>
+  </si>
+  <si>
+    <t>ET TUBE 8.0 REIN FORCED</t>
+  </si>
+  <si>
+    <t>ET TUBE 8.5 REIN FORCED</t>
+  </si>
+  <si>
+    <t>FEEDING BAG ( RMS )</t>
+  </si>
+  <si>
+    <t>FOLEYS CATHETER -2 WAY -08FR</t>
+  </si>
+  <si>
+    <t>FOLEYS CATHETER -2 WAY- 12FR</t>
+  </si>
+  <si>
+    <t>FOLEYS CATHETER -2 WAY -14FR</t>
+  </si>
+  <si>
+    <t>FOLEYS CATHETER -2 WAY- 16FR</t>
+  </si>
+  <si>
+    <t>FOLEYS CATHETER -2 WAY -18FR</t>
+  </si>
+  <si>
+    <t>GLUCI -10ML- INJ</t>
+  </si>
+  <si>
+    <t>GUEDEL AIRWAY- 0</t>
+  </si>
+  <si>
+    <t>GUEDEL AIRWAY- 00</t>
+  </si>
+  <si>
+    <t>GUEDEL AIRWAY -000</t>
+  </si>
+  <si>
+    <t>GUEDEL AIRWAY -1</t>
+  </si>
+  <si>
+    <t>GUEDEL AIRWAY -2</t>
+  </si>
+  <si>
+    <t>GUEDEL AIRWAY -3</t>
+  </si>
+  <si>
+    <t>HAEMACCEL -500ML</t>
+  </si>
+  <si>
+    <t>HEP 5000 I.U VAIL</t>
+  </si>
+  <si>
+    <t>HEPAGLAN-25000 IU INJ</t>
+  </si>
+  <si>
+    <t>HI-OXYGEN MASK -ADULT</t>
+  </si>
+  <si>
+    <t>HUMAN ACTRAPID-INJ</t>
+  </si>
+  <si>
+    <t>HUMAN MIXTARD VIAL</t>
+  </si>
+  <si>
+    <t>INFANT FEEDING TUBE -NO 10</t>
+  </si>
+  <si>
+    <t>IPRAVENT-RESPULES</t>
+  </si>
+  <si>
+    <t>IV SETS TRANS FLOW</t>
+  </si>
+  <si>
+    <t>KABILYTE FREEFLEX 500ML I.V</t>
+  </si>
+  <si>
+    <t>KABIMOL-100ML-INJ</t>
+  </si>
+  <si>
+    <t>KENADION -1ML- INJ</t>
+  </si>
+  <si>
+    <t>KETOROL INJ</t>
+  </si>
+  <si>
+    <t>KLOTIN-5ML-INJ</t>
+  </si>
+  <si>
+    <t>LANTUS SOLOSTAR 100IU INJ</t>
+  </si>
+  <si>
+    <t>LASIX 4ML INJ</t>
+  </si>
+  <si>
+    <t>LEVIPIL 5ML INJ</t>
+  </si>
+  <si>
+    <t>LEVOFLOX 100ML I.V</t>
+  </si>
+  <si>
+    <t>LIDFAST 2% 30GM JELLY</t>
+  </si>
+  <si>
+    <t>LOOZ ENEMA -275ML</t>
+  </si>
+  <si>
+    <t>LOPEZ-INJ</t>
+  </si>
+  <si>
+    <t>LOXICARD-2%-50ML-INJ</t>
+  </si>
+  <si>
+    <t>MALE CATH -LARGE</t>
+  </si>
+  <si>
+    <t>MALE CATH- MEDIUM</t>
+  </si>
+  <si>
+    <t>MALE CATH- SMALL</t>
+  </si>
+  <si>
+    <t>MEROPLAN 1GM INJ</t>
+  </si>
+  <si>
+    <t>MEROPLAN 500MG INJ</t>
+  </si>
+  <si>
+    <t>MERSILK 3-0 NW 5028</t>
+  </si>
+  <si>
+    <t>METRIS 100ML FLEXIDRIP</t>
+  </si>
+  <si>
+    <t>MEZOLAM-10ML-INJ</t>
+  </si>
+  <si>
+    <t>MICROPORE -1 INCH PLASTER</t>
+  </si>
+  <si>
+    <t>MICROPORE -3 INCH PLASTER</t>
+  </si>
+  <si>
+    <t>MUCYST-2ML-AMP</t>
+  </si>
+  <si>
+    <t>NACPHIN 10MG/1ML INJ</t>
+  </si>
+  <si>
+    <t>NASOPHARYNGEAL AIRWAY -NO 7</t>
+  </si>
+  <si>
+    <t>NEEDLE DISPOSABLE -16G</t>
+  </si>
+  <si>
+    <t>NEEDLE DISPOSABLE -18 X 1 1/2G</t>
+  </si>
+  <si>
+    <t>NEOFLON -24G</t>
+  </si>
+  <si>
+    <t>NEOFLON -26G</t>
+  </si>
+  <si>
+    <t>NEOVEC 4MG INJ</t>
+  </si>
+  <si>
+    <t>NITROCIN -5ML- INJ</t>
+  </si>
+  <si>
+    <t>NORAD-2ML-INJ</t>
+  </si>
+  <si>
+    <t>NS 0.45% 500ML</t>
+  </si>
+  <si>
+    <t>NS 100MLFLEXI DRIP</t>
+  </si>
+  <si>
+    <t>NS 500ML FLEXI DRIP</t>
+  </si>
+  <si>
+    <t>OCTRIDE-100MCG INJ</t>
+  </si>
+  <si>
+    <t>OCTRIDE-50MCG -INJ</t>
+  </si>
+  <si>
+    <t>OMNIVAN 10MLSYRINGE</t>
+  </si>
+  <si>
+    <t>OMNIVAN 2ML SYRINGE</t>
+  </si>
+  <si>
+    <t>OMNIVAN 5ML SYRINGE</t>
+  </si>
+  <si>
+    <t>OPTINEURON 3ML INJ</t>
+  </si>
+  <si>
+    <t>OXY SET ROMSONS</t>
+  </si>
+  <si>
+    <t>OXYGEN MASK -ADULT</t>
+  </si>
+  <si>
+    <t>OXYGEN MASK -PAED</t>
+  </si>
+  <si>
+    <t>OXYGEN RECOVERY KIT 60% WITH T-PIECE</t>
+  </si>
+  <si>
+    <t>PEPAR 2.25GM INJ</t>
+  </si>
+  <si>
+    <t>PEPAR -4.5GM INJ</t>
+  </si>
+  <si>
+    <t>PERINORM-INJ</t>
+  </si>
+  <si>
+    <t>PM O LINE M/F -200CM</t>
+  </si>
+  <si>
+    <t>PROFOL SPIVA 2% 50ML INJ</t>
+  </si>
+  <si>
+    <t>RL 500ML FLEXIDRIP</t>
+  </si>
+  <si>
+    <t>ROCUNIUM 50MG INJ</t>
+  </si>
+  <si>
+    <t>RYLES TUBE -NO 10 ( NG TUBE )</t>
+  </si>
+  <si>
+    <t>RYLES TUBE -NO 12 ( NG TUBE )</t>
+  </si>
+  <si>
+    <t>RYLES TUBE -NO 14 ( NG TUBE )</t>
+  </si>
+  <si>
+    <t>RYLES TUBE -NO 16 ( NG TUBE )</t>
+  </si>
+  <si>
+    <t>RYLES TUBE -NO 18 ( NG TUBE )</t>
+  </si>
+  <si>
+    <t>SERENACE 1ML INJ</t>
+  </si>
+  <si>
+    <t>SODAC-25ML-INJ</t>
+  </si>
+  <si>
+    <t>SORBITRATE-5MG-TAB</t>
+  </si>
+  <si>
+    <t>SPINAL NEEDLE -18G</t>
+  </si>
+  <si>
+    <t>SPINAL NEEDLE -20G</t>
+  </si>
+  <si>
+    <t>SPINAL NEEDLE -22G</t>
+  </si>
+  <si>
+    <t>STERILE GLOVE - 6.5-ENCORE</t>
+  </si>
+  <si>
+    <t>STERILE GLOVE -6.0-ENCORE</t>
+  </si>
+  <si>
+    <t>STERILE GLOVE -7.0-ENCORE</t>
+  </si>
+  <si>
+    <t>STERILE GLOVE -7.5-ENCORE</t>
+  </si>
+  <si>
+    <t>STERILE GLOVE- 8.0-ENCORE</t>
+  </si>
+  <si>
+    <t>SUCOL 10ML INJ</t>
+  </si>
+  <si>
+    <t>SUCTION CATHETER -NO 12</t>
+  </si>
+  <si>
+    <t>SUCTION CATHETER -NO 14</t>
+  </si>
+  <si>
+    <t>SUCTION CATHETER -NO 16</t>
+  </si>
+  <si>
+    <t>SURGEON CAPS</t>
+  </si>
+  <si>
+    <t>SURGICAL BLADE -NO 11</t>
+  </si>
+  <si>
+    <t>SURGICAL BLADE -NO 21</t>
+  </si>
+  <si>
+    <t>SURGICAL BLADE -NO 22</t>
+  </si>
+  <si>
+    <t>SYRINGE -50ML -DISPOVAN</t>
+  </si>
+  <si>
+    <t>T.T-INJ</t>
+  </si>
+  <si>
+    <t>TAXIM -1G-INJ</t>
+  </si>
+  <si>
+    <t>TEGADERM -1635- 8.5CM X 10.5CM</t>
+  </si>
+  <si>
+    <t>TEGADERM -1657R- 11.5CM X 8.5CM</t>
+  </si>
+  <si>
+    <t>TEGADERM HP PAD -8582 -5CM X 7CM</t>
+  </si>
+  <si>
+    <t>THROMBOPHOB -20GM OINT</t>
+  </si>
+  <si>
+    <t>TRANSPORE 1 INCH-PLASTER</t>
+  </si>
+  <si>
+    <t>TRANSPORE 2 INCH-PLASTER</t>
+  </si>
+  <si>
+    <t>TRANSPORE 3 INCH-PLASTER</t>
+  </si>
+  <si>
+    <t>TROPINE 1ML INJ</t>
+  </si>
+  <si>
+    <t>TROYMIDATE 20MG/10ML-INJ</t>
+  </si>
+  <si>
+    <t>TROYPOFOL-20ML-INJ</t>
+  </si>
+  <si>
+    <t>UROBAG -ROMO</t>
+  </si>
+  <si>
+    <t>UROMETER-PLUS</t>
+  </si>
+  <si>
+    <t>VACCU SUCTION SET</t>
+  </si>
+  <si>
+    <t>VASOCON- 1ML -AMP</t>
+  </si>
+  <si>
+    <t>VASOFIX -16G</t>
+  </si>
+  <si>
+    <t>VASOFIX -18G</t>
+  </si>
+  <si>
+    <t>VASOFIX- 20G</t>
+  </si>
+  <si>
+    <t>VASOFIX -22G</t>
+  </si>
+  <si>
+    <t>V-PRESS 1ML/20IU INJ</t>
+  </si>
+  <si>
+    <t>WRIST BELT -STARMED</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>vizag</t>
+  </si>
+  <si>
+    <t>Billing_Details</t>
+  </si>
+  <si>
+    <t>Rakesh Kalapala</t>
+  </si>
+  <si>
+    <t>aig</t>
+  </si>
+  <si>
+    <t>On Bill</t>
+  </si>
+  <si>
+    <t>Corporate Discount</t>
+  </si>
+  <si>
+    <t>CAPRI JALOTA</t>
+  </si>
+  <si>
+    <t>Archana</t>
   </si>
 </sst>
 </file>
@@ -245,7 +764,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm\/dd\/yyyy"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,6 +832,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF404040"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -350,7 +882,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -398,6 +930,16 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -705,7 +1247,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,7 +1294,7 @@
         <v>10015522</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>14</v>
@@ -763,7 +1305,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -783,16 +1325,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
     <col min="2" max="2" width="31.5703125" customWidth="1"/>
-    <col min="3" max="3" width="39.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -805,6 +1347,9 @@
       <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="7" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -814,7 +1359,10 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>242</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -825,7 +1373,10 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>232</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -836,7 +1387,10 @@
         <v>37</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>51</v>
+        <v>233</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -844,7 +1398,10 @@
         <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>234</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -854,6 +1411,9 @@
       <c r="C6" t="s">
         <v>30</v>
       </c>
+      <c r="D6" s="22">
+        <v>7.5</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -862,6 +1422,9 @@
       <c r="C7" t="s">
         <v>30</v>
       </c>
+      <c r="D7" s="22" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -892,7 +1455,7 @@
         <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -900,7 +1463,7 @@
         <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>235</v>
       </c>
       <c r="D12" s="10"/>
     </row>
@@ -1043,7 +1606,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1052,7 +1615,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1692,9 +2255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1708,34 +2269,34 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>54</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>59</v>
       </c>
       <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E2" s="14">
         <v>5</v>
@@ -1743,10 +2304,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E3" s="14">
         <v>5</v>
@@ -1773,7 +2334,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1783,43 +2344,1086 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B7844E7-B2C2-4511-897A-69FCDE7E1E7E}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B254"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="36" customWidth="1"/>
+    <col min="2" max="2" width="43" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="B1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B5" s="21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B6" s="21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
+      <c r="B7" s="21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B21" s="21" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B22" s="21" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B23" s="21" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B24" s="21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B25" s="21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B26" s="21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B27" s="21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B28" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B29" s="21" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B30" s="21" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B31" s="21" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B32" s="21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B33" s="21" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B34" s="21" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B35" s="21" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B36" s="21" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B37" s="21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B38" s="21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B39" s="21" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B40" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B41" s="21" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B42" s="21" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B43" s="21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B44" s="21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B45" s="21" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B46" s="21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B47" s="21" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B48" s="21" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B49" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B50" s="21" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B51" s="21" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B52" s="21" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B53" s="21" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B54" s="21" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B55" s="21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B56" s="21" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B57" s="21" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B58" s="21" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B59" s="21" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B60" s="21" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B61" s="21" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B62" s="21" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B63" s="21" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B64" s="21" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B65" s="21" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B66" s="21" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B67" s="21" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="B68" s="21" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B69" s="21" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B70" s="21" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B71" s="21" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B72" s="21" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B73" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B74" s="21" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B75" s="21" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B76" s="21" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B77" s="21" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B78" s="21" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B79" s="21" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B80" s="21" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B81" s="21" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B82" s="21" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B83" s="21" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B84" s="21" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B85" s="21" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B86" s="21" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B87" s="21" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B88" s="21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B89" s="21" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B90" s="21" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B91" s="21" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B92" s="21" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B93" s="21" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B94" s="21" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B95" s="21" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B96" s="21" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B97" s="21" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B98" s="21" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B99" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B100" s="21" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B101" s="21" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B102" s="21" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B103" s="21" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B104" s="21" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="B105" s="21" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B106" s="21" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B107" s="21" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B108" s="21" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B109" s="21" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B110" s="21" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B111" s="21" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="112" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B112" s="21" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B113" s="21" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B114" s="21" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B115" s="21" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B116" s="21" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B117" s="21" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B118" s="21" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B119" s="21" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B120" s="21" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B121" s="21" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B122" s="21" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B123" s="21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B124" s="21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="125" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B125" s="21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="126" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B126" s="21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B127" s="21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B128" s="21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B129" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B130" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B131" s="21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B132" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B133" s="21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B134" s="21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B135" s="21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B136" s="21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B137" s="21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="138" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B138" s="21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B139" s="21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="140" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B140" s="21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="141" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B141" s="21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="142" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B142" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="143" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B143" s="21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="144" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B144" s="21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="145" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B145" s="21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="146" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B146" s="21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="147" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B147" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="148" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B148" s="21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="149" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B149" s="21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="150" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B150" s="21" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="151" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B151" s="21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="152" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B152" s="21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="20"/>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="20"/>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="20"/>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="20"/>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="20"/>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="20"/>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="20"/>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="20"/>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="20"/>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="20"/>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="20"/>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="20"/>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="20"/>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="20"/>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="20"/>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="20"/>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="20"/>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="20"/>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="20"/>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="20"/>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="20"/>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="20"/>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="20"/>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="20"/>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="20"/>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="20"/>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="20"/>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="20"/>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="20"/>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="20"/>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="20"/>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="20"/>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="20"/>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="20"/>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="20"/>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="20"/>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="20"/>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="20"/>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="20"/>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="20"/>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="20"/>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="20"/>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="20"/>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="20"/>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="20"/>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="20"/>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="20"/>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" s="20"/>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" s="20"/>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" s="20"/>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" s="20"/>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" s="20"/>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" s="20"/>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" s="20"/>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" s="20"/>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" s="20"/>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="20"/>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" s="20"/>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="20"/>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" s="20"/>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" s="20"/>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" s="20"/>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" s="20"/>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" s="20"/>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" s="20"/>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" s="20"/>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" s="20"/>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" s="20"/>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" s="20"/>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" s="20"/>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" s="20"/>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" s="20"/>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" s="20"/>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" s="20"/>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" s="20"/>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" s="20"/>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" s="20"/>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" s="20"/>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" s="20"/>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" s="20"/>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" s="20"/>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" s="20"/>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
defined automation test cases for HIS regression scenarios
</commit_message>
<xml_diff>
--- a/TestData/HIS_DATA_WorkBook.xlsx
+++ b/TestData/HIS_DATA_WorkBook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10013887\Project_AIG\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79595A4-7307-4270-96EC-FC9689F17199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CA6A39-5FEB-4B5F-810F-FBE23C58A6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="227">
   <si>
     <t>Queries</t>
   </si>
@@ -208,72 +208,12 @@
     <t>Dropdown_option</t>
   </si>
   <si>
-    <t>Nikith@4744</t>
-  </si>
-  <si>
     <t>item_name</t>
   </si>
   <si>
-    <t>AVAGARD CHG 4% HAND SCRUB 500ML</t>
-  </si>
-  <si>
     <t>MICROPORE -2 INCH PLASTER</t>
   </si>
   <si>
-    <t>25% DEXTROSE 100ML</t>
-  </si>
-  <si>
-    <t>ADNEON -2ML- INJ</t>
-  </si>
-  <si>
-    <t>ALCOHOL SWABS</t>
-  </si>
-  <si>
-    <t>AMIODON 150MG INJ 3ML</t>
-  </si>
-  <si>
-    <t>ARTACIL 25MG/2.5ML INJ</t>
-  </si>
-  <si>
-    <t>ASTHALIN RESPULES</t>
-  </si>
-  <si>
-    <t>ATORVA 80MG TAB</t>
-  </si>
-  <si>
-    <t>ATRAPURE 25MG /2.5ML INJ</t>
-  </si>
-  <si>
-    <t>AUGPEN-1.2GM-INJ</t>
-  </si>
-  <si>
-    <t>AVIL-2ML-INJ</t>
-  </si>
-  <si>
-    <t>BAIN CIRCUIT- ADULT</t>
-  </si>
-  <si>
-    <t>BAIN CIRCUIT -PAED</t>
-  </si>
-  <si>
-    <t>BAND -AID ROUND</t>
-  </si>
-  <si>
-    <t>BUDECORT-0.5MG-RESPULES</t>
-  </si>
-  <si>
-    <t>CAMERA COVERS- 25CM X 2MTRS</t>
-  </si>
-  <si>
-    <t>CERTOFIX DUO -V715</t>
-  </si>
-  <si>
-    <t>CERTOFIX MONO -V315</t>
-  </si>
-  <si>
-    <t>CLOPITAB 75MG TAB</t>
-  </si>
-  <si>
     <t>CORT-S 100MG INJ</t>
   </si>
   <si>
@@ -724,18 +664,9 @@
     <t>WRIST BELT -STARMED</t>
   </si>
   <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>Single</t>
   </si>
   <si>
-    <t>vizag</t>
-  </si>
-  <si>
     <t>Billing_Details</t>
   </si>
   <si>
@@ -748,13 +679,34 @@
     <t>On Bill</t>
   </si>
   <si>
-    <t>Corporate Discount</t>
-  </si>
-  <si>
     <t>CAPRI JALOTA</t>
   </si>
   <si>
-    <t>Archana</t>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Kaandewali</t>
+  </si>
+  <si>
+    <t>Discount_Details</t>
+  </si>
+  <si>
+    <t>Patient Affordability</t>
+  </si>
+  <si>
+    <t>Good-will Discount</t>
+  </si>
+  <si>
+    <t>Aigh@1234</t>
+  </si>
+  <si>
+    <t>RajaRamChandra</t>
+  </si>
+  <si>
+    <t>AIGG.20808923</t>
   </si>
 </sst>
 </file>
@@ -882,7 +834,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -935,10 +887,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1247,7 +1196,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,7 +1240,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3">
-        <v>10015522</v>
+        <v>10014231</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>47</v>
@@ -1305,7 +1254,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>60</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -1323,10 +1272,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,9 +1284,11 @@
     <col min="2" max="2" width="31.5703125" customWidth="1"/>
     <col min="3" max="3" width="24.5703125" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>20</v>
       </c>
@@ -1348,10 +1299,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1359,13 +1313,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>242</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="E2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1373,13 +1330,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>27</v>
       </c>
@@ -1387,46 +1347,46 @@
         <v>37</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="E5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>29</v>
       </c>
       <c r="C6" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="22">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="22" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>31</v>
       </c>
@@ -1434,7 +1394,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>32</v>
       </c>
@@ -1442,7 +1402,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>33</v>
       </c>
@@ -1450,7 +1410,7 @@
         <v>8328053255</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>34</v>
       </c>
@@ -1458,16 +1418,16 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>36</v>
       </c>
@@ -1475,7 +1435,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>40</v>
       </c>
@@ -1483,7 +1443,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>38</v>
       </c>
@@ -1491,7 +1451,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>41</v>
       </c>
@@ -2255,7 +2215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="P1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2346,8 +2306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B7844E7-B2C2-4511-897A-69FCDE7E1E7E}">
   <dimension ref="A1:B254"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A142" sqref="A142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2358,819 +2318,752 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="51.75" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="B2" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B7" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B8" s="21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B9" s="21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B10" s="21" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B11" s="21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B12" s="21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B13" s="21" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="21" t="s">
+    <row r="14" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B14" s="21" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="21" t="s">
+    <row r="15" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B15" s="21" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="21" t="s">
+    <row r="16" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B16" s="21" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="21" t="s">
+    <row r="17" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B17" s="21" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="21" t="s">
+    <row r="18" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B18" s="21" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="21" t="s">
+    <row r="19" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B19" s="21" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" s="21" t="s">
+    <row r="20" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B20" s="21" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" s="21" t="s">
+    <row r="21" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B21" s="21" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="21" t="s">
+    <row r="22" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B22" s="21" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="21" t="s">
+    <row r="23" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B23" s="21" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="21" t="s">
+    <row r="24" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B24" s="21" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="21" t="s">
+    <row r="25" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B25" s="21" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="B15" s="21" t="s">
+    <row r="26" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B26" s="21" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="B16" s="21" t="s">
+    <row r="27" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B27" s="21" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="B17" s="21" t="s">
+    <row r="28" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B28" s="21" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="B18" s="21" t="s">
+    <row r="29" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B29" s="21" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19" s="21" t="s">
+    <row r="30" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B30" s="21" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="B20" s="21" t="s">
+    <row r="31" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B31" s="21" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B21" s="21" t="s">
+    <row r="32" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B32" s="21" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B22" s="21" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B23" s="21" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B24" s="21" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B25" s="21" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B26" s="21" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B27" s="21" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B28" s="21" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B29" s="21" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B30" s="21" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B31" s="21" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B32" s="21" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="33" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B33" s="21" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B34" s="21" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B35" s="21" t="s">
-        <v>145</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B36" s="21" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B37" s="21" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B38" s="21" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B39" s="21" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B40" s="21" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
     </row>
     <row r="41" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B41" s="21" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B42" s="21" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B43" s="21" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B44" s="21" t="s">
-        <v>63</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B45" s="21" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
     </row>
     <row r="46" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B46" s="21" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B47" s="21" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B48" s="21" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B49" s="21" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B50" s="21" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B51" s="21" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
     </row>
     <row r="52" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B52" s="21" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="53" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B53" s="21" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
     </row>
     <row r="54" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B54" s="21" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
     </row>
     <row r="55" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B55" s="21" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B56" s="21" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
     </row>
     <row r="57" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B57" s="21" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B58" s="21" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="59" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" ht="34.5" x14ac:dyDescent="0.25">
       <c r="B59" s="21" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="60" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B60" s="21" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="61" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B61" s="21" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B62" s="21" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="63" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B63" s="21" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
     </row>
     <row r="64" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B64" s="21" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="65" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B65" s="21" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
     </row>
     <row r="66" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B66" s="21" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
     </row>
     <row r="67" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B67" s="21" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="68" spans="2:2" ht="34.5" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B68" s="21" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
     </row>
     <row r="69" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B69" s="21" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
     </row>
     <row r="70" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B70" s="21" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
     </row>
     <row r="71" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B71" s="21" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
     </row>
     <row r="72" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B72" s="21" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
     </row>
     <row r="73" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B73" s="21" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
     </row>
     <row r="74" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B74" s="21" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
     </row>
     <row r="75" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B75" s="21" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
     </row>
     <row r="76" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B76" s="21" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
     </row>
     <row r="77" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B77" s="21" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
     </row>
     <row r="78" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B78" s="21" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="79" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B79" s="21" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="80" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B80" s="21" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
     </row>
     <row r="81" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B81" s="21" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
     <row r="82" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B82" s="21" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
     </row>
     <row r="83" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B83" s="21" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
     </row>
     <row r="84" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B84" s="21" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="85" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B85" s="21" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
     </row>
     <row r="86" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B86" s="21" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="87" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B87" s="21" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="88" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B88" s="21" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="89" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B89" s="21" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="90" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B90" s="21" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="91" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B91" s="21" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
     </row>
     <row r="92" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B92" s="21" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="93" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B93" s="21" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="94" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B94" s="21" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
     </row>
     <row r="95" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B95" s="21" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="96" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" ht="34.5" x14ac:dyDescent="0.25">
       <c r="B96" s="21" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="97" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B97" s="21" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
     </row>
     <row r="98" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B98" s="21" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
     </row>
     <row r="99" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B99" s="21" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
     <row r="100" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B100" s="21" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="101" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B101" s="21" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
     </row>
     <row r="102" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B102" s="21" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
     </row>
     <row r="103" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B103" s="21" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
     </row>
     <row r="104" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B104" s="21" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="105" spans="2:2" ht="34.5" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B105" s="21" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
     </row>
     <row r="106" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B106" s="21" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
     </row>
     <row r="107" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B107" s="21" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
     </row>
     <row r="108" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B108" s="21" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
     </row>
     <row r="109" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B109" s="21" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
     </row>
     <row r="110" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B110" s="21" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
     </row>
     <row r="111" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B111" s="21" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
     </row>
     <row r="112" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B112" s="21" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
     </row>
     <row r="113" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B113" s="21" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="114" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B114" s="21" t="s">
-        <v>223</v>
+        <v>62</v>
       </c>
     </row>
     <row r="115" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B115" s="21" t="s">
-        <v>224</v>
+        <v>63</v>
       </c>
     </row>
     <row r="116" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B116" s="21" t="s">
-        <v>225</v>
+        <v>64</v>
       </c>
     </row>
     <row r="117" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B117" s="21" t="s">
-        <v>226</v>
+        <v>65</v>
       </c>
     </row>
     <row r="118" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B118" s="21" t="s">
-        <v>227</v>
+        <v>66</v>
       </c>
     </row>
     <row r="119" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B119" s="21" t="s">
-        <v>228</v>
+        <v>67</v>
       </c>
     </row>
     <row r="120" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B120" s="21" t="s">
-        <v>229</v>
+        <v>68</v>
       </c>
     </row>
     <row r="121" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B121" s="21" t="s">
-        <v>230</v>
+        <v>69</v>
       </c>
     </row>
     <row r="122" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B122" s="21" t="s">
-        <v>231</v>
+        <v>70</v>
       </c>
     </row>
     <row r="123" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B123" s="21" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="124" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B124" s="21" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
     </row>
     <row r="125" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B125" s="21" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="126" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B126" s="21" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="127" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B127" s="21" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="128" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B128" s="21" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="129" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B129" s="21" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
     </row>
     <row r="130" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B130" s="21" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="131" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B131" s="21" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
     </row>
     <row r="132" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B132" s="21" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="133" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B133" s="21" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
     </row>
     <row r="134" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B134" s="21" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="135" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B135" s="21" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="136" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B136" s="21" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="137" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B137" s="21" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="138" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B138" s="21" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="139" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B139" s="21" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="140" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B140" s="21" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
     </row>
     <row r="141" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B141" s="21" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="142" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B142" s="21" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="143" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B143" s="21" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="144" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B144" s="21" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="145" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B145" s="21" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="146" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B146" s="21" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="147" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B147" s="21" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="148" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B148" s="21" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="149" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B149" s="21" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="150" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B150" s="21" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="151" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B151" s="21" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="152" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B152" s="21" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>